<commit_message>
added and updated results output files with charts
</commit_message>
<xml_diff>
--- a/results/04-22 node blocking/all-band-mean-pts.xlsx
+++ b/results/04-22 node blocking/all-band-mean-pts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\School\thesis\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\School\thesis\results\04-22 node blocking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -621,63 +621,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>Database</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -907,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="457955632"/>
-        <c:axId val="457954064"/>
+        <c:axId val="101264760"/>
+        <c:axId val="101511840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="457955632"/>
+        <c:axId val="101264760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,40 +875,10 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457954064"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="457954064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="60"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -982,13 +896,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Requests </a:t>
+                  <a:t>Database</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>per second</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1002,7 +911,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1026,995 +935,15 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="457955632"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>String search</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Node.js</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$C$2:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.21</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.06</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.04</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1599999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.04</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.21</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.21</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Apache/PHP</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$F$2:$F$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="457958768"/>
-        <c:axId val="457959160"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="457958768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457959160"/>
+        <c:crossAx val="101511840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="457959160"/>
+        <c:axId val="101511840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Requests </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>per second</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="457958768"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>Static file service</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Node.js</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$D$2:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.39</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.38</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.39</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.41</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.38</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.39</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.41</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.41</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Apache/PHP</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'all-band-mean-pts'!$G$2:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.56999999999999995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.53</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="346599960"/>
-        <c:axId val="346603096"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="346599960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="346603096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="346603096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0.30000000000000004"/>
+          <c:min val="60"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2130,7 +1059,1109 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346599960"/>
+        <c:crossAx val="101264760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Individual</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> bandwidths during heterogeneous testing</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Node.js</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Apache/PHP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="296046112"/>
+        <c:axId val="295422784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="296046112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>String</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> search</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="295422784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="295422784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Requests per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296046112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Node.js</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Apache/PHP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'all-band-mean-pts'!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="295783936"/>
+        <c:axId val="296040376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="295783936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Static file service</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="296040376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="296040376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.30000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="295783936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2228,63 +2259,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>Database</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2514,11 +2489,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="351627032"/>
-        <c:axId val="350009560"/>
+        <c:axId val="294333536"/>
+        <c:axId val="294330400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="351627032"/>
+        <c:axId val="294333536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2538,16 +2513,72 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Database</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350009560"/>
+        <c:crossAx val="294330400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350009560"/>
+        <c:axId val="294330400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8"/>
@@ -2661,7 +2692,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351627032"/>
+        <c:crossAx val="294333536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2766,7 +2797,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2780,7 +2811,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1200"/>
-              <a:t>String search</a:t>
+              <a:t>Individual concurrent means during</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> heterogeneous testing</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2799,7 +2834,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3045,11 +3080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="350012304"/>
-        <c:axId val="350017008"/>
+        <c:axId val="294329616"/>
+        <c:axId val="294330792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="350012304"/>
+        <c:axId val="294329616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3069,16 +3104,77 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>String</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> search</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350017008"/>
+        <c:crossAx val="294330792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350017008"/>
+        <c:axId val="294330792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3191,7 +3287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350012304"/>
+        <c:crossAx val="294329616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3575,11 +3671,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292491160"/>
-        <c:axId val="291409336"/>
+        <c:axId val="295960680"/>
+        <c:axId val="295959504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292491160"/>
+        <c:axId val="295960680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3603,12 +3699,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291409336"/>
+        <c:crossAx val="295959504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="291409336"/>
+        <c:axId val="295959504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1500"/>
@@ -3722,7 +3818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292491160"/>
+        <c:crossAx val="295960680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7146,16 +7242,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7180,14 +7276,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7211,15 +7307,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7244,14 +7340,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7276,14 +7372,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7307,15 +7403,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>771525</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7604,8 +7700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="H9" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>